<commit_message>
commit code before major change
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/ZSP_Billing_Template.xlsx
+++ b/src/main/resources/templates/ZSP_Billing_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaoyj\Desktop\ZSP\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F38170B-F8D7-4379-A673-43B87CEC654C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3634F83-34AB-488F-9E1C-6BF118EB2C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="20772" windowHeight="11232" xr2:uid="{825A4CEA-0F70-4CF0-9531-D2ED1698A1EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{825A4CEA-0F70-4CF0-9531-D2ED1698A1EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>June2024 Bill</t>
   </si>
@@ -212,10 +212,13 @@
     <t>HH 0</t>
   </si>
   <si>
-    <t>IN2407-11</t>
-  </si>
-  <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>IN2402</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -711,6 +714,84 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -724,7 +805,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
@@ -747,78 +827,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,9 +857,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -924,7 +933,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1309,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D200883C-5A4B-4BC2-A100-991DE9AF41E2}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2215,16 +2224,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90" t="s">
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J3" s="3" t="s">
@@ -2242,81 +2251,83 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="J5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
+      <c r="L5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="45">
+        <v>-10053</v>
+      </c>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="J8" s="91" t="s">
+      <c r="J8" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
+      <c r="A9" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
       <c r="J9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
+      <c r="A10" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
       <c r="J10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
+      <c r="A11" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
       <c r="J11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="6" t="s">
         <v>10</v>
       </c>
@@ -2326,17 +2337,17 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="9">
         <v>0</v>
       </c>
@@ -2347,17 +2358,17 @@
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="30">
         <v>0</v>
       </c>
@@ -2367,20 +2378,20 @@
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="13">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="13" t="str">
         <f>N39</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>17</v>
@@ -2389,17 +2400,17 @@
       <c r="R17" s="10"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="14" t="s">
         <v>18</v>
       </c>
@@ -2412,17 +2423,17 @@
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="85" t="s">
+      <c r="A19" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="14" t="s">
         <v>18</v>
       </c>
@@ -2434,15 +2445,15 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="85"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="14"/>
       <c r="L20" s="5" t="s">
         <v>22</v>
@@ -2458,45 +2469,44 @@
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="86">
+      <c r="E21" s="47">
         <v>45487</v>
       </c>
-      <c r="F21" s="87"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="18">
+      <c r="J21" s="18" t="str">
         <f>J17</f>
-        <v>0</v>
+        <v>-</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="58"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="70"/>
-      <c r="J23" s="21">
-        <f>ROUND(J15+J16+J17,2)</f>
-        <v>0</v>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -2506,42 +2516,42 @@
     </row>
     <row r="27" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="84"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="62"/>
       <c r="I28" s="22" t="s">
         <v>27</v>
       </c>
       <c r="J28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K28" s="73" t="s">
+      <c r="K28" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="74" t="s">
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="O28" s="75"/>
+      <c r="O28" s="53"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -2553,31 +2563,29 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="I30" s="19">
-        <v>0</v>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="I30" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="J30" s="19">
         <v>0</v>
       </c>
-      <c r="K30" s="79">
-        <f>ROUND(I30*J30,2)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="80">
-        <f>K30</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="81"/>
+      <c r="K30" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="O30" s="59"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
@@ -2588,8 +2596,8 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="31">
-        <v>0</v>
+      <c r="G31" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="25"/>
@@ -2603,74 +2611,72 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="31">
-        <v>0</v>
+      <c r="G32" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="N32" s="4"/>
       <c r="O32" s="25"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="59"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="62"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="66"/>
     </row>
     <row r="34" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="N34" s="61">
+      <c r="A34" s="63"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="N34" s="65">
         <v>0</v>
       </c>
-      <c r="O34" s="95"/>
+      <c r="O34" s="75"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
       <c r="H35" s="4"/>
-      <c r="N35" s="61">
-        <f>ROUND(N30+N31+N32+N33+N34,2)</f>
-        <v>0</v>
-      </c>
-      <c r="O35" s="62"/>
+      <c r="N35" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="O35" s="66"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="65"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="68"/>
     </row>
     <row r="37" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
       <c r="H37" s="17"/>
-      <c r="I37" s="32">
-        <f>N30</f>
-        <v>0</v>
+      <c r="I37" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="J37" s="33">
         <v>0.09</v>
@@ -2678,34 +2684,32 @@
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
-      <c r="N37" s="67">
-        <f>ROUND(I37*J37,2)</f>
-        <v>0</v>
-      </c>
-      <c r="O37" s="68"/>
+      <c r="N37" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="O37" s="72"/>
     </row>
     <row r="38" spans="1:15" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="69" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="20"/>
       <c r="I39" s="26"/>
       <c r="J39" s="26"/>
       <c r="K39" s="26"/>
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
-      <c r="N39" s="71">
-        <f>SUM(N35:O37)</f>
-        <v>0</v>
-      </c>
-      <c r="O39" s="72"/>
+      <c r="N39" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="O39" s="74"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="27"/>
@@ -2725,108 +2729,107 @@
       <c r="O48" s="27"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="58"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="58"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="38"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="80"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="80"/>
+      <c r="M50" s="80"/>
+      <c r="N50" s="80"/>
+      <c r="O50" s="80"/>
     </row>
     <row r="53" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="42" t="s">
+      <c r="B54" s="81"/>
+      <c r="C54" s="82"/>
+      <c r="D54" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="42" t="s">
+      <c r="E54" s="84"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="H54" s="41"/>
-      <c r="I54" s="42" t="s">
+      <c r="H54" s="82"/>
+      <c r="I54" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="J54" s="45"/>
-      <c r="K54" s="42" t="s">
+      <c r="J54" s="86"/>
+      <c r="K54" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="L54" s="46"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="47"/>
+      <c r="L54" s="87"/>
+      <c r="M54" s="81"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="88"/>
     </row>
     <row r="55" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="48">
+      <c r="A55" s="89">
         <f>E21</f>
         <v>45487</v>
       </c>
-      <c r="B55" s="49"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="51" t="str">
+      <c r="B55" s="90"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="92" t="str">
         <f>L3</f>
         <v>HH 0</v>
       </c>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="51" t="str">
+      <c r="E55" s="93"/>
+      <c r="F55" s="94"/>
+      <c r="G55" s="92" t="str">
         <f>L5</f>
-        <v>IN2407-11</v>
-      </c>
-      <c r="H55" s="54"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="55"/>
-      <c r="L55" s="56"/>
-      <c r="M55" s="56"/>
-      <c r="N55" s="56"/>
-      <c r="O55" s="57"/>
+        <v>IN2402</v>
+      </c>
+      <c r="H55" s="95"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="95"/>
+      <c r="K55" s="96"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="70"/>
+      <c r="N55" s="70"/>
+      <c r="O55" s="97"/>
     </row>
     <row r="58" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I58" s="34" t="s">
+      <c r="I58" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="J58" s="34"/>
+      <c r="J58" s="76"/>
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
-      <c r="M58" s="35">
-        <f>J23</f>
-        <v>0</v>
-      </c>
-      <c r="N58" s="36"/>
-      <c r="O58" s="37"/>
+      <c r="M58" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="N58" s="78"/>
+      <c r="O58" s="79"/>
     </row>
     <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
@@ -3001,42 +3004,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A49:O49"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N34:O34"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="M58:O58"/>
     <mergeCell ref="A50:O50"/>
@@ -3050,6 +3017,42 @@
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:O55"/>
+    <mergeCell ref="A49:O49"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>